<commit_message>
fixed | i-560 | Ajuste caja por defecto nuevo cpe - agrega caja por defecto compras
</commit_message>
<xml_diff>
--- a/public/formats/items.xlsx
+++ b/public/formats/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85497E17-63A2-40EF-8CF7-F8C6FB2567A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328A4F04-3B26-40A5-BCA4-630DA7CF89DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Código Interno</t>
   </si>
@@ -66,12 +66,6 @@
     <t>PEN</t>
   </si>
   <si>
-    <t>Coca cola</t>
-  </si>
-  <si>
-    <t>P00X</t>
-  </si>
-  <si>
     <t>Tiene Igv</t>
   </si>
   <si>
@@ -121,6 +115,18 @@
   </si>
   <si>
     <t>nombre sec 22</t>
+  </si>
+  <si>
+    <t>Código lote</t>
+  </si>
+  <si>
+    <t>Fec. Vencimiento</t>
+  </si>
+  <si>
+    <t>Pepsi Coca cola</t>
+  </si>
+  <si>
+    <t>P1212</t>
   </si>
 </sst>
 </file>
@@ -156,8 +162,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,11 +466,12 @@
     <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -484,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
@@ -499,19 +507,25 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -531,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>120.5</v>
@@ -546,24 +560,24 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>51121703</v>
@@ -572,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>150</v>
@@ -581,7 +595,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>150</v>
@@ -596,16 +610,22 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" t="s">
-        <v>31</v>
+      <c r="Q3">
+        <v>11223344</v>
+      </c>
+      <c r="R3" s="1">
+        <v>44123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó el campo para agregar un alias al producto y solo mostrarlo en los pdfs, todo esto en las cotizaciones, actualizado con master
</commit_message>
<xml_diff>
--- a/public/formats/items.xlsx
+++ b/public/formats/items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fec. Vencimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cód barras</t>
   </si>
   <si>
     <t xml:space="preserve">Producto x</t>
@@ -135,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +160,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,12 +212,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,13 +242,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
@@ -241,11 +256,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="38.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.57"/>
@@ -309,19 +324,22 @@
       <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>20202020</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>120.25</v>
@@ -330,7 +348,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>120.5</v>
@@ -345,33 +363,36 @@
         <v>1</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>10000001</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>51121703</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>150</v>
@@ -380,7 +401,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>150</v>
@@ -395,16 +416,16 @@
         <v>1</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>11223344</v>
@@ -412,6 +433,12 @@
       <c r="S3" s="1" t="n">
         <v>44123</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <v>10000002</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S8" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>